<commit_message>
Dont remeber if changed anything in code
</commit_message>
<xml_diff>
--- a/2025 Knights Attendance and Game Locations.xlsx
+++ b/2025 Knights Attendance and Game Locations.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="116">
   <si>
     <t xml:space="preserve">When do you plan to travel, be out of town for work/etc.. reasons, or have other occasions? Please let us know </t>
   </si>
@@ -47,6 +47,9 @@
     <t>J</t>
   </si>
   <si>
+    <t>x</t>
+  </si>
+  <si>
     <t>Charlie</t>
   </si>
   <si>
@@ -77,6 +80,9 @@
     <t>Eric</t>
   </si>
   <si>
+    <t>I</t>
+  </si>
+  <si>
     <t xml:space="preserve">Denis </t>
   </si>
   <si>
@@ -107,9 +113,6 @@
     <t>Devin</t>
   </si>
   <si>
-    <t>I</t>
-  </si>
-  <si>
     <t>Brennen</t>
   </si>
   <si>
@@ -128,6 +131,9 @@
     <t>A</t>
   </si>
   <si>
+    <t xml:space="preserve"> A</t>
+  </si>
+  <si>
     <t>Attending Field Players</t>
   </si>
   <si>
@@ -137,9 +143,6 @@
     <t>Noah</t>
   </si>
   <si>
-    <t>In</t>
-  </si>
-  <si>
     <t>Ryan</t>
   </si>
   <si>
@@ -210,9 +213,6 @@
   </si>
   <si>
     <t>total</t>
-  </si>
-  <si>
-    <t>Column 1</t>
   </si>
   <si>
     <t>Date</t>
@@ -967,261 +967,8 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr lvl="0">
-              <a:defRPr b="0">
-                <a:solidFill>
-                  <a:srgbClr val="757575"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr b="0">
-                <a:solidFill>
-                  <a:srgbClr val="757575"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-              </a:rPr>
-              <a:t>Distribution of Squad Size on Game Days</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="stacked"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Attendance!$D$49</c:f>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln cmpd="sng">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-          <c:cat>
-            <c:strRef>
-              <c:f>Attendance!$C$50:$C$56</c:f>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Attendance!$D$50:$D$56</c:f>
-              <c:numCache/>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:overlap val="100"/>
-        <c:axId val="290548745"/>
-        <c:axId val="1142226479"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="290548745"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr lvl="0">
-                  <a:defRPr b="0">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                  </a:rPr>
-                  <a:t>Attended Field</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:spPr/>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr lvl="0">
-              <a:defRPr b="0">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1142226479"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="1142226479"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="B7B7B7"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:minorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="CCCCCC">
-                  <a:alpha val="0"/>
-                </a:srgbClr>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:minorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr lvl="0">
-                  <a:defRPr b="0">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                  </a:rPr>
-                  <a:t>Times</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr lvl="0">
-              <a:defRPr b="0">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="290548745"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:txPr>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr lvl="0">
-            <a:defRPr b="0">
-              <a:solidFill>
-                <a:srgbClr val="1A1A1A"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-            </a:defRPr>
-          </a:pPr>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-  </c:chart>
-</c:chartSpace>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>952500</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="5715000" cy="3533775"/>
-    <xdr:graphicFrame>
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="1" name="Chart 1" title="Chart"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData fLocksWithSheet="0"/>
-  </xdr:oneCellAnchor>
-</xdr:wsDr>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1231,7 +978,7 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:G15" displayName="Table1" name="Table1" id="1">
   <tableColumns count="7">
-    <tableColumn name="Column 1" id="1"/>
+    <tableColumn name="x" id="1"/>
     <tableColumn name="Date" id="2"/>
     <tableColumn name="Time" id="3"/>
     <tableColumn name="Opponent" id="4"/>
@@ -1472,7 +1219,6 @@
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
     </row>
     <row r="2">
       <c r="A2" s="1"/>
@@ -1489,7 +1235,6 @@
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
     </row>
     <row r="4">
       <c r="A4" s="2"/>
@@ -1513,41 +1258,38 @@
         <v>45817.0</v>
       </c>
       <c r="I4" s="4">
-        <v>45824.0</v>
+        <v>45826.0</v>
       </c>
       <c r="J4" s="4">
-        <v>45826.0</v>
+        <v>45466.0</v>
       </c>
       <c r="K4" s="4">
-        <v>45466.0</v>
+        <v>45838.0</v>
       </c>
       <c r="L4" s="4">
-        <v>45838.0</v>
+        <v>45845.0</v>
       </c>
       <c r="M4" s="4">
-        <v>45845.0</v>
+        <v>45852.0</v>
       </c>
       <c r="N4" s="4">
-        <v>45852.0</v>
+        <v>45859.0</v>
       </c>
       <c r="O4" s="4">
-        <v>45859.0</v>
+        <v>45866.0</v>
       </c>
       <c r="P4" s="4">
-        <v>45866.0</v>
+        <v>45873.0</v>
       </c>
       <c r="Q4" s="4">
-        <v>45873.0</v>
-      </c>
-      <c r="R4" s="4">
         <v>45880.0</v>
       </c>
-      <c r="S4" s="5"/>
+      <c r="R4" s="4"/>
+      <c r="S4" s="4"/>
       <c r="T4" s="5"/>
       <c r="U4" s="5"/>
       <c r="V4" s="5"/>
       <c r="W4" s="5"/>
-      <c r="X4" s="5"/>
     </row>
     <row r="5">
       <c r="A5" s="6"/>
@@ -1564,18 +1306,17 @@
       <c r="F5" s="8"/>
       <c r="G5" s="8"/>
       <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="9" t="s">
+      <c r="I5" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="K5" s="8"/>
-      <c r="L5" s="9"/>
-      <c r="M5" s="8"/>
-      <c r="N5" s="9"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="9"/>
+      <c r="N5" s="8"/>
       <c r="O5" s="8"/>
       <c r="P5" s="8"/>
       <c r="Q5" s="8"/>
-      <c r="R5" s="8"/>
     </row>
     <row r="6">
       <c r="A6" s="10"/>
@@ -1594,7 +1335,7 @@
       </c>
       <c r="G6" s="8"/>
       <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
+      <c r="I6" s="9"/>
       <c r="J6" s="9"/>
       <c r="K6" s="9"/>
       <c r="L6" s="9"/>
@@ -1603,7 +1344,6 @@
       <c r="O6" s="9"/>
       <c r="P6" s="9"/>
       <c r="Q6" s="9"/>
-      <c r="R6" s="9"/>
     </row>
     <row r="7">
       <c r="A7" s="10"/>
@@ -1620,18 +1360,15 @@
       <c r="F7" s="8"/>
       <c r="G7" s="8"/>
       <c r="H7" s="8"/>
-      <c r="I7" s="9" t="s">
-        <v>6</v>
-      </c>
+      <c r="I7" s="8"/>
       <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
+      <c r="K7" s="9"/>
       <c r="L7" s="9"/>
-      <c r="M7" s="9"/>
+      <c r="M7" s="8"/>
       <c r="N7" s="8"/>
       <c r="O7" s="8"/>
       <c r="P7" s="8"/>
       <c r="Q7" s="8"/>
-      <c r="R7" s="8"/>
     </row>
     <row r="8">
       <c r="A8" s="10"/>
@@ -1657,9 +1394,12 @@
       <c r="M8" s="8"/>
       <c r="N8" s="8"/>
       <c r="O8" s="8"/>
-      <c r="P8" s="8"/>
-      <c r="Q8" s="9"/>
-      <c r="R8" s="9"/>
+      <c r="P8" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q8" s="9" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="10"/>
@@ -1670,7 +1410,7 @@
         <v>7</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E9" s="9"/>
       <c r="F9" s="8"/>
@@ -1680,14 +1420,13 @@
       <c r="J9" s="9"/>
       <c r="K9" s="9"/>
       <c r="L9" s="9"/>
-      <c r="M9" s="9"/>
-      <c r="N9" s="9" t="s">
+      <c r="M9" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="O9" s="8"/>
-      <c r="P9" s="9"/>
+      <c r="N9" s="8"/>
+      <c r="O9" s="9"/>
+      <c r="P9" s="8"/>
       <c r="Q9" s="8"/>
-      <c r="R9" s="8"/>
     </row>
     <row r="10">
       <c r="A10" s="10"/>
@@ -1698,24 +1437,23 @@
         <v>7</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E10" s="8"/>
       <c r="F10" s="8"/>
       <c r="G10" s="8"/>
       <c r="H10" s="8"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9" t="s">
+      <c r="I10" s="9" t="s">
         <v>6</v>
       </c>
+      <c r="J10" s="8"/>
       <c r="K10" s="8"/>
-      <c r="L10" s="8"/>
+      <c r="L10" s="9"/>
       <c r="M10" s="9"/>
-      <c r="N10" s="9"/>
+      <c r="N10" s="8"/>
       <c r="O10" s="8"/>
       <c r="P10" s="8"/>
       <c r="Q10" s="8"/>
-      <c r="R10" s="8"/>
     </row>
     <row r="11">
       <c r="A11" s="10"/>
@@ -1726,7 +1464,7 @@
         <v>7</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E11" s="8"/>
       <c r="F11" s="8"/>
@@ -1737,11 +1475,12 @@
       <c r="K11" s="8"/>
       <c r="L11" s="8"/>
       <c r="M11" s="8"/>
-      <c r="N11" s="8"/>
+      <c r="N11" s="9" t="s">
+        <v>6</v>
+      </c>
       <c r="O11" s="8"/>
       <c r="P11" s="8"/>
       <c r="Q11" s="8"/>
-      <c r="R11" s="8"/>
     </row>
     <row r="12">
       <c r="A12" s="10"/>
@@ -1752,28 +1491,29 @@
         <v>7</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E12" s="8"/>
       <c r="F12" s="9"/>
       <c r="G12" s="9"/>
       <c r="H12" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="I12" s="9"/>
-      <c r="J12" s="9"/>
+        <v>16</v>
+      </c>
+      <c r="I12" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="J12" s="9" t="s">
+        <v>6</v>
+      </c>
       <c r="K12" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="L12" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="M12" s="9"/>
-      <c r="N12" s="8"/>
-      <c r="O12" s="9"/>
-      <c r="P12" s="8"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="8"/>
+      <c r="N12" s="9"/>
+      <c r="O12" s="8"/>
+      <c r="P12" s="9"/>
       <c r="Q12" s="9"/>
-      <c r="R12" s="9"/>
     </row>
     <row r="13">
       <c r="A13" s="10"/>
@@ -1781,10 +1521,10 @@
         <v>9.0</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E13" s="9" t="s">
         <v>6</v>
@@ -1792,29 +1532,28 @@
       <c r="F13" s="9"/>
       <c r="G13" s="9"/>
       <c r="H13" s="9"/>
-      <c r="I13" s="9"/>
+      <c r="I13" s="8"/>
       <c r="J13" s="8"/>
       <c r="K13" s="8"/>
       <c r="L13" s="8"/>
-      <c r="M13" s="8"/>
+      <c r="M13" s="9"/>
       <c r="N13" s="9"/>
       <c r="O13" s="9"/>
-      <c r="P13" s="9"/>
+      <c r="P13" s="8"/>
       <c r="Q13" s="8"/>
-      <c r="R13" s="8"/>
     </row>
     <row r="14">
       <c r="A14" s="14" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B14" s="6">
         <v>10.0</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E14" s="9" t="s">
         <v>6</v>
@@ -1851,9 +1590,6 @@
         <v>6</v>
       </c>
       <c r="Q14" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="R14" s="9" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1863,10 +1599,10 @@
         <v>11.0</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E15" s="8"/>
       <c r="F15" s="9"/>
@@ -1874,18 +1610,21 @@
         <v>6</v>
       </c>
       <c r="H15" s="9"/>
-      <c r="I15" s="9"/>
-      <c r="J15" s="9"/>
+      <c r="I15" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="J15" s="9" t="s">
+        <v>22</v>
+      </c>
       <c r="K15" s="9"/>
       <c r="L15" s="9"/>
       <c r="M15" s="9"/>
       <c r="N15" s="9"/>
       <c r="O15" s="9"/>
-      <c r="P15" s="9"/>
-      <c r="Q15" s="9" t="s">
+      <c r="P15" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="R15" s="9"/>
+      <c r="Q15" s="9"/>
     </row>
     <row r="16">
       <c r="A16" s="10"/>
@@ -1893,10 +1632,10 @@
         <v>12.0</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
@@ -1910,8 +1649,7 @@
       <c r="N16" s="8"/>
       <c r="O16" s="8"/>
       <c r="P16" s="8"/>
-      <c r="Q16" s="8"/>
-      <c r="R16" s="9"/>
+      <c r="Q16" s="9"/>
     </row>
     <row r="17">
       <c r="A17" s="10"/>
@@ -1919,10 +1657,10 @@
         <v>13.0</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E17" s="9" t="s">
         <v>6</v>
@@ -1933,15 +1671,14 @@
       <c r="G17" s="9"/>
       <c r="H17" s="8"/>
       <c r="I17" s="8"/>
-      <c r="J17" s="8"/>
+      <c r="J17" s="9"/>
       <c r="K17" s="8"/>
       <c r="L17" s="8"/>
       <c r="M17" s="8"/>
       <c r="N17" s="8"/>
-      <c r="O17" s="8"/>
-      <c r="P17" s="9"/>
-      <c r="Q17" s="8"/>
-      <c r="R17" s="9"/>
+      <c r="O17" s="9"/>
+      <c r="P17" s="8"/>
+      <c r="Q17" s="9"/>
     </row>
     <row r="18">
       <c r="A18" s="10"/>
@@ -1949,10 +1686,10 @@
         <v>14.0</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E18" s="9"/>
       <c r="F18" s="9" t="s">
@@ -1960,60 +1697,54 @@
       </c>
       <c r="G18" s="8"/>
       <c r="H18" s="8"/>
-      <c r="I18" s="8"/>
+      <c r="I18" s="9"/>
       <c r="J18" s="9"/>
-      <c r="K18" s="9"/>
-      <c r="L18" s="8"/>
-      <c r="M18" s="9" t="s">
+      <c r="K18" s="8"/>
+      <c r="L18" s="9" t="s">
         <v>6</v>
       </c>
+      <c r="M18" s="8"/>
       <c r="N18" s="8"/>
       <c r="O18" s="8"/>
       <c r="P18" s="8"/>
       <c r="Q18" s="8"/>
-      <c r="R18" s="8"/>
     </row>
     <row r="19">
       <c r="A19" s="14" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B19" s="10">
         <v>15.0</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D19" s="16" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E19" s="9"/>
       <c r="F19" s="9"/>
       <c r="G19" s="9" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="H19" s="8"/>
       <c r="I19" s="8"/>
-      <c r="J19" s="8"/>
-      <c r="K19" s="8"/>
-      <c r="L19" s="8"/>
+      <c r="J19" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="K19" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="L19" s="9" t="s">
+        <v>6</v>
+      </c>
       <c r="M19" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="N19" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="O19" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="P19" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q19" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="R19" s="9" t="s">
-        <v>6</v>
-      </c>
+      <c r="N19" s="9"/>
+      <c r="O19" s="9"/>
+      <c r="P19" s="9"/>
+      <c r="Q19" s="9"/>
     </row>
     <row r="20">
       <c r="A20" s="10"/>
@@ -2021,14 +1752,14 @@
         <v>16.0</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E20" s="9"/>
       <c r="F20" s="9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G20" s="9"/>
       <c r="H20" s="8"/>
@@ -2040,8 +1771,7 @@
       <c r="N20" s="8"/>
       <c r="O20" s="8"/>
       <c r="P20" s="8"/>
-      <c r="Q20" s="8"/>
-      <c r="R20" s="9"/>
+      <c r="Q20" s="9"/>
     </row>
     <row r="21">
       <c r="A21" s="10"/>
@@ -2049,10 +1779,10 @@
         <v>17.0</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E21" s="8"/>
       <c r="F21" s="8"/>
@@ -2060,18 +1790,17 @@
       <c r="H21" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="I21" s="8"/>
+      <c r="I21" s="9"/>
       <c r="J21" s="9"/>
-      <c r="K21" s="9"/>
+      <c r="K21" s="8"/>
       <c r="L21" s="8"/>
       <c r="M21" s="8"/>
       <c r="N21" s="8"/>
-      <c r="O21" s="8"/>
-      <c r="P21" s="9"/>
+      <c r="O21" s="9"/>
+      <c r="P21" s="9" t="s">
+        <v>6</v>
+      </c>
       <c r="Q21" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="R21" s="9" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2081,35 +1810,46 @@
         <v>18.0</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="G22" s="9" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="H22" s="9" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="I22" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="J22" s="8"/>
-      <c r="K22" s="8"/>
-      <c r="L22" s="8"/>
-      <c r="M22" s="9"/>
-      <c r="N22" s="9"/>
-      <c r="O22" s="8"/>
+        <v>22</v>
+      </c>
+      <c r="J22" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="K22" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="L22" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="M22" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="N22" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="O22" s="9" t="s">
+        <v>22</v>
+      </c>
       <c r="P22" s="8"/>
       <c r="Q22" s="8"/>
-      <c r="R22" s="8"/>
     </row>
     <row r="23">
       <c r="A23" s="10"/>
@@ -2117,27 +1857,26 @@
         <v>19.0</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D23" s="13" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E23" s="8"/>
       <c r="F23" s="8"/>
       <c r="G23" s="9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H23" s="8"/>
-      <c r="I23" s="9"/>
+      <c r="I23" s="8"/>
       <c r="J23" s="8"/>
       <c r="K23" s="8"/>
       <c r="L23" s="8"/>
       <c r="M23" s="8"/>
       <c r="N23" s="8"/>
-      <c r="O23" s="8"/>
-      <c r="P23" s="9"/>
+      <c r="O23" s="9"/>
+      <c r="P23" s="8"/>
       <c r="Q23" s="8"/>
-      <c r="R23" s="8"/>
     </row>
     <row r="24">
       <c r="A24" s="10"/>
@@ -2145,10 +1884,10 @@
         <v>20.0</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D24" s="13" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E24" s="9" t="s">
         <v>6</v>
@@ -2158,16 +1897,17 @@
       <c r="H24" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="I24" s="9"/>
+      <c r="I24" s="9" t="s">
+        <v>6</v>
+      </c>
       <c r="J24" s="8"/>
       <c r="K24" s="8"/>
       <c r="L24" s="8"/>
       <c r="M24" s="8"/>
       <c r="N24" s="8"/>
-      <c r="O24" s="8"/>
-      <c r="P24" s="9"/>
+      <c r="O24" s="9"/>
+      <c r="P24" s="8"/>
       <c r="Q24" s="8"/>
-      <c r="R24" s="8"/>
     </row>
     <row r="25">
       <c r="A25" s="10"/>
@@ -2175,58 +1915,60 @@
         <v>21.0</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E25" s="8"/>
       <c r="F25" s="9"/>
       <c r="G25" s="9" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="H25" s="8"/>
-      <c r="I25" s="8"/>
+      <c r="I25" s="9" t="s">
+        <v>29</v>
+      </c>
       <c r="J25" s="8"/>
       <c r="K25" s="8"/>
       <c r="L25" s="8"/>
       <c r="M25" s="8"/>
-      <c r="N25" s="8"/>
+      <c r="N25" s="9"/>
       <c r="O25" s="9"/>
-      <c r="P25" s="9"/>
-      <c r="Q25" s="8"/>
-      <c r="R25" s="9"/>
+      <c r="P25" s="8"/>
+      <c r="Q25" s="9"/>
     </row>
     <row r="26">
       <c r="B26" s="6">
         <v>22.0</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F26" s="9" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G26" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="H26" s="9"/>
-      <c r="I26" s="8"/>
-      <c r="J26" s="8"/>
-      <c r="K26" s="8"/>
+        <v>38</v>
+      </c>
+      <c r="H26" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="I26" s="9"/>
+      <c r="J26" s="9"/>
+      <c r="K26" s="9"/>
       <c r="L26" s="8"/>
       <c r="M26" s="8"/>
       <c r="N26" s="8"/>
       <c r="O26" s="8"/>
       <c r="P26" s="8"/>
       <c r="Q26" s="8"/>
-      <c r="R26" s="8"/>
     </row>
     <row r="27">
       <c r="A27" s="17"/>
@@ -2252,17 +1994,16 @@
       <c r="U27" s="17"/>
       <c r="V27" s="17"/>
       <c r="W27" s="17"/>
-      <c r="X27" s="17"/>
     </row>
     <row r="28">
       <c r="A28" s="18"/>
       <c r="B28" s="18"/>
       <c r="C28" s="18" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D28" s="19"/>
       <c r="E28" s="8">
-        <f t="shared" ref="E28:R28" si="1">countif(E6:E26, "")</f>
+        <f t="shared" ref="E28:Q28" si="1">countif(E6:E26, "")</f>
         <v>15</v>
       </c>
       <c r="F28" s="8">
@@ -2275,27 +2016,27 @@
       </c>
       <c r="H28" s="8">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I28" s="8">
         <f t="shared" si="1"/>
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="J28" s="8">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="K28" s="8">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="L28" s="8">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="M28" s="8">
         <f t="shared" si="1"/>
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="N28" s="8">
         <f t="shared" si="1"/>
@@ -2307,22 +2048,18 @@
       </c>
       <c r="P28" s="8">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="Q28" s="8">
         <f t="shared" si="1"/>
-        <v>17</v>
-      </c>
-      <c r="R28" s="8">
-        <f t="shared" si="1"/>
         <v>18</v>
       </c>
+      <c r="R28" s="8"/>
       <c r="S28" s="8"/>
       <c r="T28" s="8"/>
       <c r="U28" s="8"/>
       <c r="V28" s="8"/>
       <c r="W28" s="8"/>
-      <c r="X28" s="8"/>
     </row>
     <row r="29">
       <c r="A29" s="8"/>
@@ -2330,40 +2067,40 @@
       <c r="C29" s="8"/>
       <c r="D29" s="8"/>
       <c r="E29" s="20">
-        <f t="shared" ref="E29:R29" si="2">E28/(COUNTA($D$6:$D$26))</f>
+        <f>E28/(COUNTA($D$6:$D$26) - countif($E$6:$E$26, "A"))</f>
+        <v>0.75</v>
+      </c>
+      <c r="F29" s="20">
+        <f t="shared" ref="F29:Q29" si="2">F28/(COUNTA($D$6:$D$26) - countif(F$6:F$26, "A"))</f>
+        <v>0.7</v>
+      </c>
+      <c r="G29" s="20">
+        <f t="shared" si="2"/>
+        <v>0.7</v>
+      </c>
+      <c r="H29" s="20">
+        <f t="shared" si="2"/>
         <v>0.7142857143</v>
       </c>
-      <c r="F29" s="20">
+      <c r="I29" s="20">
         <f t="shared" si="2"/>
         <v>0.6666666667</v>
       </c>
-      <c r="G29" s="20">
-        <f t="shared" si="2"/>
-        <v>0.6666666667</v>
-      </c>
-      <c r="H29" s="20">
+      <c r="J29" s="20">
         <f t="shared" si="2"/>
         <v>0.7619047619</v>
       </c>
-      <c r="I29" s="20">
-        <f t="shared" si="2"/>
-        <v>0.8571428571</v>
-      </c>
-      <c r="J29" s="20">
-        <f t="shared" si="2"/>
-        <v>0.9047619048</v>
-      </c>
       <c r="K29" s="20">
         <f t="shared" si="2"/>
-        <v>0.9047619048</v>
+        <v>0.8095238095</v>
       </c>
       <c r="L29" s="20">
         <f t="shared" si="2"/>
-        <v>0.9047619048</v>
+        <v>0.8095238095</v>
       </c>
       <c r="M29" s="20">
         <f t="shared" si="2"/>
-        <v>0.8571428571</v>
+        <v>0.8095238095</v>
       </c>
       <c r="N29" s="20">
         <f t="shared" si="2"/>
@@ -2375,22 +2112,18 @@
       </c>
       <c r="P29" s="20">
         <f t="shared" si="2"/>
-        <v>0.9047619048</v>
+        <v>0.8095238095</v>
       </c>
       <c r="Q29" s="20">
         <f t="shared" si="2"/>
-        <v>0.8095238095</v>
-      </c>
-      <c r="R29" s="20">
-        <f t="shared" si="2"/>
         <v>0.8571428571</v>
       </c>
+      <c r="R29" s="8"/>
       <c r="S29" s="8"/>
       <c r="T29" s="8"/>
       <c r="U29" s="8"/>
       <c r="V29" s="8"/>
       <c r="W29" s="8"/>
-      <c r="X29" s="8"/>
     </row>
     <row r="30">
       <c r="A30" s="21"/>
@@ -2399,7 +2132,7 @@
         <v>7</v>
       </c>
       <c r="E30" s="22">
-        <f t="shared" ref="E30:R30" si="3">COUNTIFS($C$5:$C$26, "D", E5:E26, "")</f>
+        <f t="shared" ref="E30:Q30" si="3">COUNTIFS($C$5:$C$26, "D", E5:E26, "")</f>
         <v>7</v>
       </c>
       <c r="F30" s="22">
@@ -2416,7 +2149,7 @@
       </c>
       <c r="I30" s="22">
         <f t="shared" si="3"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J30" s="22">
         <f t="shared" si="3"/>
@@ -2428,11 +2161,11 @@
       </c>
       <c r="L30" s="22">
         <f t="shared" si="3"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M30" s="22">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="N30" s="22">
         <f t="shared" si="3"/>
@@ -2444,25 +2177,21 @@
       </c>
       <c r="P30" s="22">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="Q30" s="22">
         <f t="shared" si="3"/>
-        <v>7</v>
-      </c>
-      <c r="R30" s="22">
-        <f t="shared" si="3"/>
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="21"/>
       <c r="B31" s="21"/>
       <c r="C31" s="21" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E31" s="22">
-        <f t="shared" ref="E31:R31" si="4">COUNTIFS($C$5:$C$26, "M", E5:E26, "")</f>
+        <f t="shared" ref="E31:Q31" si="4">COUNTIFS($C$5:$C$26, "M", E5:E26, "")</f>
         <v>3</v>
       </c>
       <c r="F31" s="22">
@@ -2475,15 +2204,15 @@
       </c>
       <c r="H31" s="22">
         <f t="shared" si="4"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I31" s="22">
         <f t="shared" si="4"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J31" s="22">
         <f t="shared" si="4"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K31" s="22">
         <f t="shared" si="4"/>
@@ -2491,11 +2220,11 @@
       </c>
       <c r="L31" s="22">
         <f t="shared" si="4"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="M31" s="22">
         <f t="shared" si="4"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="N31" s="22">
         <f t="shared" si="4"/>
@@ -2507,13 +2236,9 @@
       </c>
       <c r="P31" s="22">
         <f t="shared" si="4"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="Q31" s="22">
-        <f t="shared" si="4"/>
-        <v>5</v>
-      </c>
-      <c r="R31" s="22">
         <f t="shared" si="4"/>
         <v>6</v>
       </c>
@@ -2522,10 +2247,10 @@
       <c r="A32" s="21"/>
       <c r="B32" s="21"/>
       <c r="C32" s="21" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E32" s="22">
-        <f t="shared" ref="E32:R32" si="5">COUNTIFS($C$5:$C$26, "F", E5:E26, "")</f>
+        <f t="shared" ref="E32:Q32" si="5">COUNTIFS($C$5:$C$26, "F", E5:E26, "")</f>
         <v>5</v>
       </c>
       <c r="F32" s="22">
@@ -2542,23 +2267,23 @@
       </c>
       <c r="I32" s="22">
         <f t="shared" si="5"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="J32" s="22">
         <f t="shared" si="5"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="K32" s="22">
         <f t="shared" si="5"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="L32" s="22">
         <f t="shared" si="5"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="M32" s="22">
         <f t="shared" si="5"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="N32" s="22">
         <f t="shared" si="5"/>
@@ -2574,11 +2299,7 @@
       </c>
       <c r="Q32" s="22">
         <f t="shared" si="5"/>
-        <v>5</v>
-      </c>
-      <c r="R32" s="22">
-        <f t="shared" si="5"/>
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="33">
@@ -2587,19 +2308,16 @@
     </row>
     <row r="34">
       <c r="A34" s="21" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B34" s="21">
         <v>23.0</v>
       </c>
       <c r="C34" s="21" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D34" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="H34" s="21" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="35">
@@ -2610,143 +2328,143 @@
         <v>4</v>
       </c>
       <c r="D35" s="21" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="21"/>
       <c r="B38" s="21"/>
       <c r="C38" s="21" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E38" s="23">
-        <f>AVERAGE(E27:R28)</f>
-        <v>17.35714286</v>
+        <f>AVERAGE(E27:Q28)</f>
+        <v>16.23076923</v>
       </c>
       <c r="F38" s="24" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G38" s="25">
         <f>E38-1.96*(F40)</f>
-        <v>16.38022463</v>
+        <v>15.3116126</v>
       </c>
       <c r="H38" s="25">
         <f>E38+1.96*(F40)</f>
-        <v>18.33406109</v>
-      </c>
-      <c r="J38" s="21" t="s">
-        <v>45</v>
+        <v>17.14992586</v>
+      </c>
+      <c r="I38" s="21" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="21"/>
       <c r="B39" s="21"/>
       <c r="C39" s="21" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E39" s="26">
-        <f>median(E28:R28)</f>
-        <v>18</v>
-      </c>
-      <c r="J39" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="K39" s="21"/>
-      <c r="L39" s="21" t="s">
+        <f>median(E28:Q28)</f>
+        <v>17</v>
+      </c>
+      <c r="I39" s="21" t="s">
         <v>48</v>
+      </c>
+      <c r="J39" s="21"/>
+      <c r="K39" s="21" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="21"/>
       <c r="B40" s="21"/>
       <c r="C40" s="21" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E40" s="27">
-        <f>STDEV(E28:R28)</f>
-        <v>1.86494557</v>
+        <f>STDEV(E28:Q28)</f>
+        <v>1.690850188</v>
       </c>
       <c r="F40" s="26">
-        <f>E40/sqrt(countA(E28:R28))</f>
-        <v>0.4984276691</v>
-      </c>
-      <c r="J40" s="21" t="s">
-        <v>50</v>
-      </c>
-      <c r="K40" s="21"/>
-      <c r="L40" s="21" t="s">
+        <f>E40/sqrt(countA(E28:Q28))</f>
+        <v>0.4689574656</v>
+      </c>
+      <c r="I40" s="21" t="s">
         <v>51</v>
       </c>
+      <c r="J40" s="21"/>
+      <c r="K40" s="21" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="41">
-      <c r="J41" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="K41" s="21"/>
-      <c r="L41" s="21" t="s">
+      <c r="I41" s="21" t="s">
         <v>53</v>
+      </c>
+      <c r="J41" s="21"/>
+      <c r="K41" s="21" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="21"/>
       <c r="B42" s="21"/>
       <c r="C42" s="21" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E42" s="28">
-        <f>average(E29:R29)</f>
-        <v>0.8265306122</v>
+        <f>average(E29:Q29)</f>
+        <v>0.7807692308</v>
       </c>
       <c r="F42" s="24" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G42" s="29">
         <f>E42-1.96*(F44)</f>
-        <v>0.7800106965</v>
+        <v>0.741652005</v>
       </c>
       <c r="H42" s="29">
         <f>E42+1.96*(F44)</f>
-        <v>0.873050528</v>
-      </c>
-      <c r="J42" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="K42" s="21"/>
-      <c r="L42" s="21" t="s">
+        <v>0.8198864565</v>
+      </c>
+      <c r="I42" s="21" t="s">
         <v>56</v>
+      </c>
+      <c r="J42" s="21"/>
+      <c r="K42" s="21" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="21"/>
       <c r="B43" s="21"/>
       <c r="C43" s="21" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E43" s="28">
-        <f>median(E29:R29)</f>
-        <v>0.8571428571</v>
-      </c>
-      <c r="J43" s="21" t="s">
-        <v>58</v>
-      </c>
-      <c r="K43" s="21"/>
-      <c r="L43" s="21" t="s">
+        <f>median(E29:Q29)</f>
+        <v>0.8095238095</v>
+      </c>
+      <c r="I43" s="21" t="s">
         <v>59</v>
+      </c>
+      <c r="J43" s="21"/>
+      <c r="K43" s="21" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="21"/>
       <c r="B44" s="21"/>
       <c r="C44" s="21" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E44" s="26">
-        <f>STDEV(E29:R29)</f>
-        <v>0.08880693189</v>
+        <f>STDEV(E29:Q29)</f>
+        <v>0.07195875679</v>
       </c>
       <c r="F44" s="26">
-        <f>E44/sqrt(countA(E28:R28))</f>
-        <v>0.02373465091</v>
+        <f>E44/sqrt(countA(E28:Q28))</f>
+        <v>0.01995776825</v>
       </c>
     </row>
     <row r="45">
@@ -2756,15 +2474,14 @@
       <c r="A46" s="31"/>
       <c r="B46" s="31"/>
       <c r="C46" s="31" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D46" s="31">
         <f>COUNTA(D6:D25)</f>
         <v>20</v>
       </c>
       <c r="H46" s="31"/>
-      <c r="I46" s="31"/>
-      <c r="J46" s="32"/>
+      <c r="I46" s="32"/>
     </row>
     <row r="47">
       <c r="A47" s="31"/>
@@ -2774,14 +2491,14 @@
     </row>
     <row r="48">
       <c r="A48" s="31" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B48" s="31"/>
       <c r="C48" s="31" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D48" s="31" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H48" s="31"/>
     </row>
@@ -2792,16 +2509,16 @@
       </c>
       <c r="B49" s="34"/>
       <c r="C49" s="34">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("sort(unique(TRANSPOSE(E28:R28)))"),14.0)</f>
+        <f t="array" ref="C49:C54">sort(unique(TRANSPOSE(E28:Q28)))</f>
         <v>14</v>
       </c>
       <c r="D49" s="8">
-        <f t="shared" ref="D49:D56" si="7">countif($E$28:$R$28, C49)</f>
-        <v>2</v>
+        <f t="shared" ref="D49:D56" si="7">countif($E$28:$Q$28, C49)</f>
+        <v>3</v>
       </c>
       <c r="E49" s="28">
         <f t="shared" ref="E49:E56" si="8">D49/$D$57</f>
-        <v>0.1428571429</v>
+        <v>0.2307692308</v>
       </c>
       <c r="G49" s="35"/>
       <c r="H49" s="36"/>
@@ -2813,16 +2530,15 @@
       </c>
       <c r="B50" s="8"/>
       <c r="C50" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),15.0)</f>
-        <v>15</v>
+        <v>15.0</v>
       </c>
       <c r="D50" s="8">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E50" s="28">
         <f t="shared" si="8"/>
-        <v>0.07142857143</v>
+        <v>0.1538461538</v>
       </c>
       <c r="G50" s="35"/>
       <c r="H50" s="36"/>
@@ -2834,8 +2550,7 @@
       </c>
       <c r="B51" s="8"/>
       <c r="C51" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),16.0)</f>
-        <v>16</v>
+        <v>16.0</v>
       </c>
       <c r="D51" s="8">
         <f t="shared" si="7"/>
@@ -2843,7 +2558,7 @@
       </c>
       <c r="E51" s="28">
         <f t="shared" si="8"/>
-        <v>0.07142857143</v>
+        <v>0.07692307692</v>
       </c>
       <c r="G51" s="35"/>
       <c r="H51" s="36"/>
@@ -2855,16 +2570,15 @@
       </c>
       <c r="B52" s="8"/>
       <c r="C52" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),17.0)</f>
-        <v>17</v>
+        <v>17.0</v>
       </c>
       <c r="D52" s="8">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E52" s="28">
         <f t="shared" si="8"/>
-        <v>0.07142857143</v>
+        <v>0.3076923077</v>
       </c>
       <c r="G52" s="35"/>
       <c r="H52" s="36"/>
@@ -2876,16 +2590,15 @@
       </c>
       <c r="B53" s="8"/>
       <c r="C53" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),18.0)</f>
-        <v>18</v>
+        <v>18.0</v>
       </c>
       <c r="D53" s="8">
         <f t="shared" si="7"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E53" s="28">
         <f t="shared" si="8"/>
-        <v>0.2857142857</v>
+        <v>0.1538461538</v>
       </c>
       <c r="G53" s="35"/>
       <c r="H53" s="36"/>
@@ -2897,16 +2610,15 @@
       </c>
       <c r="B54" s="8"/>
       <c r="C54" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),19.0)</f>
-        <v>19</v>
+        <v>19.0</v>
       </c>
       <c r="D54" s="8">
         <f t="shared" si="7"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E54" s="28">
         <f t="shared" si="8"/>
-        <v>0.3571428571</v>
+        <v>0.07692307692</v>
       </c>
       <c r="G54" s="35"/>
       <c r="H54" s="36"/>
@@ -2935,17 +2647,14 @@
     </row>
     <row r="57">
       <c r="C57" s="37" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D57" s="38">
         <f>SUM(D49:D54)</f>
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="H45:I45"/>
-  </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
@@ -2971,7 +2680,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="39" t="s">
-        <v>66</v>
+        <v>11</v>
       </c>
       <c r="B1" s="40" t="s">
         <v>67</v>

</xml_diff>